<commit_message>
update to julia 1.11
</commit_message>
<xml_diff>
--- a/examples/SBB/model_parsing_diagnostics.SBB_case3.xlsx
+++ b/examples/SBB/model_parsing_diagnostics.SBB_case3.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="608">
   <si>
     <t>label</t>
   </si>
@@ -903,7 +903,7 @@
     <t>dependence</t>
   </si>
   <si>
-    <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4,TNH4,TMn,TFe,TH2S,FeS,CH4,H,TH3PO4,THF,TCO2,Ca</t>
+    <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4,TNH4,TMn,TFe,TH2S,FeS,CH4,H,TH3PO4,THF,TCO2,Ca,CaCO3,MnCO3,FeCO3</t>
   </si>
   <si>
     <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4</t>
@@ -912,7 +912,7 @@
     <t>O2,Age,POC,NO2,TNH4,TMn,TFe,TH2S,FeS,CH4</t>
   </si>
   <si>
-    <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4,CH4,TCO2,H,Ca,TMn,TFe,TH3PO4,THF</t>
+    <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4,CH4,TCO2,H,Ca,CaCO3,TMn,MnCO3,TFe,FeCO3,TH3PO4,THF</t>
   </si>
   <si>
     <t>O2,Age,POC,NO2,NO3,MnO2,FeOOH,THSO4,TNH4,TH2S</t>
@@ -930,13 +930,13 @@
     <t>MnO2,NO3,NO2,O2,Age,POC,TMn,TFe,TH2S</t>
   </si>
   <si>
-    <t>MnO2,NO3,NO2,O2,Age,POC,TMn,TFe,TH2S,TCO2,H</t>
+    <t>MnO2,NO3,NO2,O2,Age,POC,TMn,TFe,TH2S,TCO2,H,MnCO3</t>
   </si>
   <si>
     <t>FeOOH,MnO2,NO3,NO2,O2,Age,POC,TFe,FeS,TH2S</t>
   </si>
   <si>
-    <t>FeOOH,MnO2,NO3,NO2,O2,Age,POC,TFe,TH2S,H,TCO2</t>
+    <t>FeOOH,MnO2,NO3,NO2,O2,Age,POC,TFe,TH2S,H,FeS,TCO2,FeCO3</t>
   </si>
   <si>
     <t>THSO4,FeOOH,MnO2,NO3,NO2,O2,Age,POC,TH2S,FeS,CH4</t>
@@ -954,16 +954,19 @@
     <t>FeS,TH2S</t>
   </si>
   <si>
-    <t>TCO2,H,Ca</t>
-  </si>
-  <si>
-    <t>TCO2,H,Ca,TH3PO4,THF</t>
-  </si>
-  <si>
-    <t>TCO2,H,TMn</t>
-  </si>
-  <si>
-    <t>TCO2,H,TFe</t>
+    <t>TCO2,H,Ca,CaCO3</t>
+  </si>
+  <si>
+    <t>TCO2,H,Ca,CaCO3,TH3PO4,THF</t>
+  </si>
+  <si>
+    <t>TCO2,H,TMn,MnCO3</t>
+  </si>
+  <si>
+    <t>TCO2,H,TFe,FeCO3</t>
+  </si>
+  <si>
+    <t>H4SiO4,BSi</t>
   </si>
   <si>
     <t>TH3PO4,H,THF,TCO2,Ca</t>
@@ -1701,7 +1704,7 @@
     <t>reaction rate</t>
   </si>
   <si>
-    <t>S_O2,S_TCO2,S_TNH4,S_TH3PO4,S_NO2,S_NO3,S_TMn,S_TFe,S_THSO4,S_TH2S,S_CH4,S_Ca,S_H4SiO4,S_TA,S_TA,S_TA</t>
+    <t>S_O2,S_TCO2,S_TNH4,S_TH3PO4,S_NO2,S_NO3,S_TMn,S_TFe,S_THSO4,S_TH2S,S_CH4,S_Ca,S_H4SiO4,S_TA,S_TA,S_TA,RCaCO3_pre,RMnCO3_pre,RFeCO3_pre</t>
   </si>
   <si>
     <t>S_TNH4,S_TA</t>
@@ -1813,6 +1816,39 @@
   </si>
   <si>
     <t>kFeSH2S</t>
+  </si>
+  <si>
+    <t>kFeSdis</t>
+  </si>
+  <si>
+    <t>kFeSpre</t>
+  </si>
+  <si>
+    <t>kCaCO3dis</t>
+  </si>
+  <si>
+    <t>kCaCO3pre</t>
+  </si>
+  <si>
+    <t>kMnCO3dis</t>
+  </si>
+  <si>
+    <t>kMnCO3pre</t>
+  </si>
+  <si>
+    <t>kFeCO3dis</t>
+  </si>
+  <si>
+    <t>kFeCO3pre</t>
+  </si>
+  <si>
+    <t>kBSidis</t>
+  </si>
+  <si>
+    <t>kASipre</t>
+  </si>
+  <si>
+    <t>kCFA_pre</t>
   </si>
   <si>
     <t>kMo_rm2</t>
@@ -12721,7 +12757,7 @@
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -12729,7 +12765,7 @@
         <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -12737,7 +12773,7 @@
         <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -12745,7 +12781,7 @@
         <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -12753,7 +12789,7 @@
         <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -12761,7 +12797,7 @@
         <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -12769,7 +12805,7 @@
         <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -12787,7 +12823,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
         <v>222</v>
@@ -12795,1666 +12831,1666 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" t="s">
         <v>317</v>
-      </c>
-      <c r="B3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B12" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B14" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B15" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B16" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B17" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B20" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B21" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B22" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B25" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B27" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B28" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B29" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B30" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B33" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B34" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
+        <v>351</v>
+      </c>
+      <c r="B35" t="s">
         <v>350</v>
-      </c>
-      <c r="B35" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B36" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B37" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B38" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B39" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B41" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B42" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B43" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B44" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B45" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B46" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B47" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B48" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B49" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B50" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B51" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B52" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B53" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B54" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B55" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B56" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B57" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B58" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B60" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B61" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B62" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B63" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B65" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B66" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B67" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B68" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B69" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B70" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B71" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B72" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B73" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B74" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B75" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B76" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B77" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B78" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B79" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
+        <v>397</v>
+      </c>
+      <c r="B80" t="s">
         <v>396</v>
-      </c>
-      <c r="B80" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B81" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B82" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B83" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B84" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B85" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B86" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B87" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B88" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B89" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B90" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B91" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B92" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B93" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B94" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B95" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B96" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B97" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B98" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B99" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B100" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B101" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B102" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B103" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B104" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B105" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B106" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B107" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B108" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B109" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B110" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B111" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B112" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B113" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B114" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B115" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B116" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B117" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B118" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B119" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B120" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B121" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B122" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B123" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B124" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B125" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B126" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B127" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B128" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B129" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B130" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B131" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B132" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B133" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B134" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B135" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B136" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B137" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B138" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B139" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B140" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B142" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B143" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B144" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B145" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B146" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B147" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B148" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B149" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B150" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B151" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B152" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B153" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B154" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B155" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B156" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B157" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B158" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B159" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B160" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B161" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B162" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B163" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B164" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B165" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B166" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B167" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B168" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B169" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B170" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
+        <v>489</v>
+      </c>
+      <c r="B171" t="s">
         <v>488</v>
-      </c>
-      <c r="B171" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B172" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B173" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B174" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B175" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B176" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B177" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B178" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B179" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B180" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B181" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B182" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B183" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B184" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B185" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B186" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B187" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B188" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B189" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B190" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B191" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B192" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B193" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B194" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B195" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B196" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B197" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B198" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B199" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B200" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
+        <v>521</v>
+      </c>
+      <c r="B201" t="s">
         <v>520</v>
-      </c>
-      <c r="B201" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B202" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B203" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B204" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B205" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B206" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B207" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B208" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B209" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -14464,7 +14500,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -14472,7 +14508,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
         <v>222</v>
@@ -14483,43 +14519,43 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C3" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B4" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C4" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B5" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C5" t="s">
         <v>232</v>
@@ -14527,112 +14563,112 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C6" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C7" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C8" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B9" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B10" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B11" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C11" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B12" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B13" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C13" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B14" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C14" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B15" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C15" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -14640,10 +14676,10 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C16" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -14651,117 +14687,117 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C17" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B18" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C18" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B19" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C19" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>564</v>
+      </c>
+      <c r="B20" t="s">
+        <v>556</v>
+      </c>
+      <c r="C20" t="s">
         <v>563</v>
-      </c>
-      <c r="B20" t="s">
-        <v>555</v>
-      </c>
-      <c r="C20" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B21" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C21" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B22" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C22" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B23" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C23" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B24" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C24" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C25" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B26" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C26" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B27" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -14769,10 +14805,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B28" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C28" t="s">
         <v>77</v>
@@ -14780,10 +14816,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B29" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C29" t="s">
         <v>79</v>
@@ -14791,10 +14827,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B30" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C30" t="s">
         <v>80</v>
@@ -14802,10 +14838,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B31" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
@@ -14813,10 +14849,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B32" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C32" t="s">
         <v>85</v>
@@ -14824,10 +14860,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B33" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C33" t="s">
         <v>87</v>
@@ -14835,10 +14871,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B34" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C34" t="s">
         <v>88</v>
@@ -14846,10 +14882,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B35" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -14857,10 +14893,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B36" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C36" t="s">
         <v>92</v>
@@ -14868,10 +14904,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B37" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C37" t="s">
         <v>93</v>
@@ -14879,10 +14915,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B38" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C38" t="s">
         <v>96</v>
@@ -14890,10 +14926,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B39" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C39" t="s">
         <v>99</v>
@@ -14901,10 +14937,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B40" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C40" t="s">
         <v>100</v>
@@ -14912,10 +14948,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B41" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C41" t="s">
         <v>100</v>
@@ -14923,10 +14959,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B42" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C42" t="s">
         <v>101</v>
@@ -14934,10 +14970,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B43" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C43" t="s">
         <v>102</v>
@@ -14945,10 +14981,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B44" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C44" t="s">
         <v>103</v>
@@ -14956,10 +14992,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B45" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C45" t="s">
         <v>104</v>
@@ -14967,13 +15003,145 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B46" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C46" t="s">
-        <v>595</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>596</v>
+      </c>
+      <c r="B47" t="s">
+        <v>556</v>
+      </c>
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>597</v>
+      </c>
+      <c r="B48" t="s">
+        <v>556</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>598</v>
+      </c>
+      <c r="B49" t="s">
+        <v>556</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>599</v>
+      </c>
+      <c r="B50" t="s">
+        <v>556</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>600</v>
+      </c>
+      <c r="B51" t="s">
+        <v>556</v>
+      </c>
+      <c r="C51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>601</v>
+      </c>
+      <c r="B52" t="s">
+        <v>556</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>602</v>
+      </c>
+      <c r="B53" t="s">
+        <v>556</v>
+      </c>
+      <c r="C53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>603</v>
+      </c>
+      <c r="B54" t="s">
+        <v>556</v>
+      </c>
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>604</v>
+      </c>
+      <c r="B55" t="s">
+        <v>556</v>
+      </c>
+      <c r="C55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>552</v>
+      </c>
+      <c r="B56" t="s">
+        <v>556</v>
+      </c>
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>605</v>
+      </c>
+      <c r="B57" t="s">
+        <v>556</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>606</v>
+      </c>
+      <c r="B58" t="s">
+        <v>556</v>
+      </c>
+      <c r="C58" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>